<commit_message>
Adding elements, pages and tests
</commit_message>
<xml_diff>
--- a/travelResults.xlsx
+++ b/travelResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isvendsen\projects\FinnTraining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A654A6-86AE-448F-BBF9-A3B9505860E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD6251B-76F7-435F-A3B2-A59E9AA65CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{14C59F66-184E-4EBC-A017-C58ED963DCB4}"/>
   </bookViews>
@@ -36,12 +36,171 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>799 kr</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="55">
   <si>
     <t>796 kr</t>
+  </si>
+  <si>
+    <t>ma. 06.11</t>
+  </si>
+  <si>
+    <t>ti. 07.11</t>
+  </si>
+  <si>
+    <t>on. 08.11</t>
+  </si>
+  <si>
+    <t>to. 09.11</t>
+  </si>
+  <si>
+    <t>fr. 10.11</t>
+  </si>
+  <si>
+    <t>lø. 11.11</t>
+  </si>
+  <si>
+    <t>sø. 12.11</t>
+  </si>
+  <si>
+    <t>1 029 kr</t>
+  </si>
+  <si>
+    <t>995 kr</t>
+  </si>
+  <si>
+    <t>961 kr</t>
+  </si>
+  <si>
+    <t>Søk</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>1 487 kr</t>
+  </si>
+  <si>
+    <t>1 277 kr</t>
+  </si>
+  <si>
+    <t>1 415 kr</t>
+  </si>
+  <si>
+    <t>1 807 kr</t>
+  </si>
+  <si>
+    <t>1 497 kr</t>
+  </si>
+  <si>
+    <t>1 523 kr</t>
+  </si>
+  <si>
+    <t>1 722 kr</t>
+  </si>
+  <si>
+    <t>1 223 kr</t>
+  </si>
+  <si>
+    <t>986 kr</t>
+  </si>
+  <si>
+    <t>945 kr</t>
+  </si>
+  <si>
+    <t>1 140 kr</t>
+  </si>
+  <si>
+    <t>1 475 kr</t>
+  </si>
+  <si>
+    <t>930 kr</t>
+  </si>
+  <si>
+    <t>896 kr</t>
+  </si>
+  <si>
+    <t>1 026 kr</t>
+  </si>
+  <si>
+    <t>925 kr</t>
+  </si>
+  <si>
+    <t>934 kr</t>
+  </si>
+  <si>
+    <t>966 kr</t>
+  </si>
+  <si>
+    <t>1 439 kr</t>
+  </si>
+  <si>
+    <t>809 kr</t>
+  </si>
+  <si>
+    <t>1 045 kr</t>
+  </si>
+  <si>
+    <t>933 kr</t>
+  </si>
+  <si>
+    <t>789 kr</t>
+  </si>
+  <si>
+    <t>813 kr</t>
+  </si>
+  <si>
+    <t>1 050 kr</t>
+  </si>
+  <si>
+    <t>1 125 kr</t>
+  </si>
+  <si>
+    <t>ma. 13.11</t>
+  </si>
+  <si>
+    <t>ti. 14.11</t>
+  </si>
+  <si>
+    <t>on. 15.11</t>
+  </si>
+  <si>
+    <t>to. 16.11</t>
+  </si>
+  <si>
+    <t>898 kr</t>
+  </si>
+  <si>
+    <t>1 220 kr</t>
+  </si>
+  <si>
+    <t>1 538 kr</t>
+  </si>
+  <si>
+    <t>1 957 kr</t>
+  </si>
+  <si>
+    <t>2 052 kr</t>
+  </si>
+  <si>
+    <t>1 000 kr</t>
+  </si>
+  <si>
+    <t>1 514 kr</t>
+  </si>
+  <si>
+    <t>941 kr</t>
+  </si>
+  <si>
+    <t>775 kr</t>
+  </si>
+  <si>
+    <t>937 kr</t>
+  </si>
+  <si>
+    <t>1 357 kr</t>
+  </si>
+  <si>
+    <t>771 kr</t>
   </si>
 </sst>
 </file>
@@ -394,60 +553,191 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51F63E2F-22BF-4E46-B320-A4D1273E0603}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A8" sqref="A8:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" t="s">
         <v>0</v>
       </c>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="F6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>8</v>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>